<commit_message>
cleaned and optimized for SKU number naming
</commit_message>
<xml_diff>
--- a/reference.xlsx
+++ b/reference.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F2F1395-C4DF-41E8-B161-3349D2A5280A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\GitHub\Project-Angel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2249A5AA-9F10-4F9E-8E12-B9A174EF7521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,43 +36,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>SKU</t>
   </si>
   <si>
-    <t>Associated Patch</t>
+    <t>A</t>
   </si>
   <si>
-    <t>TS-CRACK-BLK-L</t>
+    <t>B</t>
   </si>
   <si>
-    <t>TS-CRACK-BLK</t>
-  </si>
-  <si>
-    <t>TS-CRACK-BLK-XL</t>
-  </si>
-  <si>
-    <t>TS-BIGDAWG-BLK-S</t>
-  </si>
-  <si>
-    <t>TS-BIGDAWG-BLK</t>
-  </si>
-  <si>
-    <t>TS-BIGDAWG-BLK-M</t>
-  </si>
-  <si>
-    <t>TS-YAP-BLK-2XL</t>
-  </si>
-  <si>
-    <t>TS-YAP-BLK-3XL</t>
+    <t>PATCH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,65 +422,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>9</v>
       </c>
     </row>

</xml_diff>